<commit_message>
edit typos (CBM thickness, VEGF165:NRP1 binding affinity in [Soker, 1998] & delete outliers and ELISA IC50
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F81789-5025-574A-859F-ABDF8E993892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7EC385-627D-414D-A732-82B663E7EE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18440" yWindow="700" windowWidth="44800" windowHeight="22920" activeTab="3" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22920" activeTab="4" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="VEGFA165_VEGFR2" sheetId="4" r:id="rId4"/>
     <sheet name="VEGFA165_NRP1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -78,6 +78,83 @@
         </r>
       </text>
     </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{869334AA-FFFD-AE45-94B9-ED3218882153}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Upper limit = 167.655
+Lower limit = 74.513</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{64054238-CC51-B445-B187-AE09C29B0B3E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Upper limit = 279.086
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lower limit = 108.383</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -126,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="39">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -239,10 +316,10 @@
     <t>Fuh2000</t>
   </si>
   <si>
-    <t>ELISA</t>
-  </si>
-  <si>
     <t>Pan2007</t>
+  </si>
+  <si>
+    <t>dr = r/(2A)*dA</t>
   </si>
 </sst>
 </file>
@@ -518,9 +595,6 @@
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -556,6 +630,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,10 +648,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -876,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C9A479-2AA3-884B-8FF7-FA729F57839B}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,19 +961,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1"/>
@@ -919,22 +992,22 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
-        <v>44.99</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="D2" s="3">
-        <v>65.8</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1.84</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="B2" s="2">
+        <v>44.993898209967412</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.5468244269792875</v>
+      </c>
+      <c r="D2" s="2">
+        <v>65.795246424795408</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1.838396591281048</v>
+      </c>
+      <c r="G2" s="23" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -954,7 +1027,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -966,10 +1039,10 @@
       <c r="D3" s="1">
         <v>80</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>5.3</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
@@ -991,7 +1064,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -1003,10 +1076,10 @@
       <c r="D4" s="1">
         <v>83</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>3</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1028,7 +1101,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
@@ -1040,10 +1113,10 @@
       <c r="D5" s="1">
         <v>82</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>3.5</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="23" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1063,22 +1136,22 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
-        <v>28.77</v>
-      </c>
-      <c r="C6" s="12">
+      <c r="B6" s="11">
+        <v>28.76813695875796</v>
+      </c>
+      <c r="C6" s="11">
         <v>1.0622081338618323</v>
       </c>
-      <c r="D6" s="12">
-        <v>52.93</v>
-      </c>
-      <c r="E6" s="13">
+      <c r="D6" s="11">
+        <v>52.925674284012274</v>
+      </c>
+      <c r="E6" s="12">
         <v>0.45708536881646961</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1100,7 +1173,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G7" s="2"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1119,6 +1192,11 @@
       <c r="L7" s="1">
         <f t="shared" si="1"/>
         <v>0.45708536881646961</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1154,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1166,41 +1244,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>69</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>5.5</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="1">
@@ -1209,15 +1287,15 @@
       <c r="C3" s="1">
         <v>12.5</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="1">
@@ -1226,15 +1304,15 @@
       <c r="C4" s="1">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1">
@@ -1243,15 +1321,15 @@
       <c r="C5" s="1">
         <v>18.899999999999999</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1">
@@ -1260,49 +1338,49 @@
       <c r="C6" s="1">
         <v>14.17</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1">
-        <v>61.87</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1">
-        <v>1.33</v>
+        <v>6.64</v>
       </c>
       <c r="D7" s="1">
-        <v>68.13</v>
-      </c>
-      <c r="E7" s="10">
-        <v>1.66</v>
+        <v>68</v>
+      </c>
+      <c r="E7" s="9">
+        <v>12.1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>55.67</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1">
-        <v>1.04</v>
+        <v>7.32</v>
       </c>
       <c r="D8" s="1">
-        <v>57.82</v>
-      </c>
-      <c r="E8" s="10">
-        <v>1.24</v>
+        <v>58</v>
+      </c>
+      <c r="E8" s="9">
+        <v>6.57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1">
@@ -1316,12 +1394,12 @@
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="1">
@@ -1334,28 +1412,28 @@
       <c r="D10" s="1">
         <v>113.4</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <f>B10*2/100</f>
         <v>1.78</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>103.38</v>
       </c>
-      <c r="C11" s="12">
-        <f>(194.26-67.23)/3.92</f>
-        <v>32.405612244897959</v>
-      </c>
-      <c r="D11" s="12">
+      <c r="C11" s="11">
+        <f>(167.655-74.513)/3.92</f>
+        <v>23.760714285714286</v>
+      </c>
+      <c r="D11" s="11">
         <v>139.87</v>
       </c>
-      <c r="E11" s="13">
-        <f>(314.612-95.553)/3.92</f>
-        <v>55.882397959183685</v>
+      <c r="E11" s="12">
+        <f>(279.086-108.383)/3.92</f>
+        <v>43.546683673469396</v>
       </c>
     </row>
   </sheetData>
@@ -1366,10 +1444,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,86 +1457,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>16</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="1">
         <v>9</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="1">
-        <v>196</v>
-      </c>
-      <c r="D5" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="12">
+      <c r="C5" s="11">
         <v>7.5</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D5" s="12">
         <v>3</v>
       </c>
     </row>
@@ -1471,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C5"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1482,16 +1546,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G1" t="s">
@@ -1508,17 +1572,17 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <f>AVERAGE(I2:I5)</f>
         <v>230</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <f>STDEVA(I2:I5)/SQRT(4)</f>
         <v>60.964470527239605</v>
       </c>
@@ -1536,7 +1600,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1545,7 +1609,7 @@
       <c r="C3" s="1">
         <v>339</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G3" t="s">
@@ -1562,7 +1626,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1571,7 +1635,7 @@
       <c r="C4" s="1">
         <v>760</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G4" t="s">
@@ -1588,7 +1652,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1597,7 +1661,7 @@
       <c r="C5" s="1">
         <v>770</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G5" t="s">
@@ -1614,7 +1678,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1623,7 +1687,7 @@
       <c r="C6" s="1">
         <v>37.1</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>4.9000000000000004</v>
       </c>
       <c r="G6" t="s">
@@ -1640,7 +1704,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1649,7 +1713,7 @@
       <c r="C7" s="1">
         <v>51.7</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>5.8</v>
       </c>
       <c r="G7" t="s">
@@ -1666,16 +1730,16 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <v>9.8000000000000007</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>0.4</v>
       </c>
       <c r="G8" t="s">
@@ -1740,10 +1804,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1752,35 +1816,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3">
-        <v>2090</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="2">
+        <v>2.09</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1789,12 +1853,12 @@
       <c r="C3" s="1">
         <v>0.2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1803,26 +1867,26 @@
       <c r="C4" s="1">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="1">
-        <v>0.23</v>
-      </c>
-      <c r="D5" s="10" t="s">
+        <v>0.32</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1831,78 +1895,50 @@
       <c r="C6" s="1">
         <v>113</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <f>C6*0.35</f>
         <v>39.549999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>36</v>
+      <c r="A7" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1">
         <v>120</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>36</v>
+      <c r="A8" s="14" t="s">
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1">
         <v>25</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1">
-        <v>120</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="C9" s="11">
         <v>25</v>
       </c>
-      <c r="D10" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="12">
-        <v>25</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="D9" s="12">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit SE -> SD in capillary basement membrane thickness and add more notes
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7EC385-627D-414D-A732-82B663E7EE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB90E4E-3423-4A49-9875-D81ED9766470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22920" activeTab="4" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     <author>Yunjeong Lee</author>
   </authors>
   <commentList>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{EE5AAFA1-5D10-C347-87DD-F3889D416BA5}">
       <text>
         <r>
           <rPr>
@@ -74,84 +74,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>We need to check for accuracy</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{869334AA-FFFD-AE45-94B9-ED3218882153}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yunjeong Lee:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Upper limit = 167.655
-Lower limit = 74.513</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{64054238-CC51-B445-B187-AE09C29B0B3E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yunjeong Lee:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Upper limit = 279.086
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Lower limit = 108.383</t>
+          <t>All references show mean+/-SE values</t>
         </r>
       </text>
     </comment>
@@ -165,6 +88,710 @@
     <author>Yunjeong Lee</author>
   </authors>
   <commentList>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{C4AAA6B2-9BD9-1746-AF06-F09AA047F1D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SD not SE</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{57820837-87CC-154D-ABDA-2F7B7F8DAB0C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">SD = 12.5 nm
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>n = 100</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{268D93CA-546C-014C-BD5E-79D88978D419}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">SD = 16 nm
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>n = 8</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{BECC8C1A-53BD-B344-8091-D3346FF7CCDC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SD = 18.90</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{C5458797-ECBF-C24D-B558-39DD5A3F08D9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SD = 14.17</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{2A46D8DF-C71C-DB4B-97D6-6C1414099FF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Yunjeong Lee:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculated from 95% CI of total wall thickness and endothelial cell thickness (n=4)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{7E6B9E3B-D048-FF44-B063-87A613674E19}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculated from 95% CI of total wall thickness and endothelial cell thickness (n=4)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{632CA213-3BB7-0745-AF20-0BE8597213A8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Yunjeong Lee:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Calculated from 95% CI of total wall thickness and endothelial cell thickness (n=3)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{D0891471-D081-7D49-A638-FDD2E6BE6EA6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Calculated from 95% CI of total wall thickness and endothelial cell thickness (n=5)
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{64BEA8E4-9BD4-734F-93FA-A8843F7785E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>I caluclated using upper and lower limit.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{5B8BC328-C175-1645-944D-85396FC5B1C5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">SE
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">n = 4
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>=&gt; SD = SE*sqrt(4)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">We need to check for accuracy
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">n = 4
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SD = SE * sqrt(n)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{869334AA-FFFD-AE45-94B9-ED3218882153}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Calculated SE using
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">95% percentile: 194.26
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5% percentile: 67.23
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Accuracy of calculation is unknown</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{64054238-CC51-B445-B187-AE09C29B0B3E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Calculated SE using
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">95% percentile: 314.612
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>5% percentile: 95.553</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yunjeong Lee</author>
+  </authors>
+  <commentList>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{F5752615-28CF-6E4E-A51C-5229D569314F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SE?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yunjeong Lee</author>
+  </authors>
+  <commentList>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SE?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yunjeong Lee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>SE?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yunjeong Lee</author>
+  </authors>
+  <commentList>
     <comment ref="D6" authorId="0" shapeId="0" xr:uid="{E2BBAABC-FA0C-8F40-98A9-9861430A0343}">
       <text>
         <r>
@@ -203,7 +830,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="39">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -316,10 +943,10 @@
     <t>Fuh2000</t>
   </si>
   <si>
-    <t>Pan2007</t>
-  </si>
-  <si>
     <t>dr = r/(2A)*dA</t>
+  </si>
+  <si>
+    <t>Lean SD</t>
   </si>
 </sst>
 </file>
@@ -946,11 +1573,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C9A479-2AA3-884B-8FF7-FA729F57839B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C9A479-2AA3-884B-8FF7-FA729F57839B}">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1196,7 +1823,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1225,6 +1852,7 @@
     <mergeCell ref="G5:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1233,7 +1861,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1251,7 +1879,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>7</v>
@@ -1353,13 +1981,15 @@
         <v>62</v>
       </c>
       <c r="C7" s="1">
-        <v>6.64</v>
+        <f>6.64/1.96*SQRT(4)</f>
+        <v>6.7755102040816322</v>
       </c>
       <c r="D7" s="1">
         <v>68</v>
       </c>
       <c r="E7" s="9">
-        <v>12.1</v>
+        <f>12.1/1.96*SQRT(4)</f>
+        <v>12.346938775510203</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1370,13 +2000,15 @@
         <v>56</v>
       </c>
       <c r="C8" s="1">
-        <v>7.32</v>
+        <f>7.32/1.96*SQRT(3)</f>
+        <v>6.4686795466347871</v>
       </c>
       <c r="D8" s="1">
         <v>58</v>
       </c>
       <c r="E8" s="9">
-        <v>6.57</v>
+        <f>6.57/1.96*SQRT(5)</f>
+        <v>7.4953911286600103</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1406,15 +2038,15 @@
         <v>89</v>
       </c>
       <c r="C10" s="1">
-        <f>B10*2.2/100</f>
-        <v>1.9580000000000002</v>
+        <f>B10*2.2/100*2</f>
+        <v>3.9160000000000004</v>
       </c>
       <c r="D10" s="1">
         <v>113.4</v>
       </c>
       <c r="E10" s="9">
-        <f>B10*2/100</f>
-        <v>1.78</v>
+        <f>B10*2/100*2</f>
+        <v>3.56</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1425,15 +2057,15 @@
         <v>103.38</v>
       </c>
       <c r="C11" s="11">
-        <f>(167.655-74.513)/3.92</f>
-        <v>23.760714285714286</v>
+        <f>(194.26-67.23)/3.29</f>
+        <v>38.610942249240118</v>
       </c>
       <c r="D11" s="11">
         <v>139.87</v>
       </c>
       <c r="E11" s="12">
-        <f>(279.086-108.383)/3.92</f>
-        <v>43.546683673469396</v>
+        <f>(314.612-95.553)/3.29</f>
+        <v>66.58328267477205</v>
       </c>
     </row>
   </sheetData>
@@ -1443,11 +2075,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68B970-3B91-2544-A9A4-014D1F0CD0C8}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1528,15 +2160,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6BC7D1-10B3-434D-851C-DD9B7FABFD43}">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1799,15 +2432,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1902,43 +2536,29 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="1">
-        <v>120</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="11">
         <v>25</v>
       </c>
-      <c r="D8" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="11">
-        <v>25</v>
-      </c>
-      <c r="D9" s="12">
+      <c r="D8" s="12">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
In "CBM thickness" sheet, "Obese SE" -> "Obese SD"
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB90E4E-3423-4A49-9875-D81ED9766470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA35D195-482B-DB4E-9E90-022C6F878887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22920" activeTab="4" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22400" windowHeight="22920" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -830,7 +830,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="40">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -947,6 +947,9 @@
   </si>
   <si>
     <t>Lean SD</t>
+  </si>
+  <si>
+    <t>Obese SD</t>
   </si>
 </sst>
 </file>
@@ -1860,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1885,7 +1888,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -2440,7 +2443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
delete "-" in cells
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA35D195-482B-DB4E-9E90-022C6F878887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A99B3A8-86B0-544D-A779-9EFF33D362F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22400" windowHeight="22920" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22920" activeTab="4" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -830,7 +830,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="40">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -1580,7 +1580,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1700,9 +1700,7 @@
       <c r="B4" s="1">
         <v>42</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1">
         <v>83</v>
       </c>
@@ -1863,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1901,12 +1899,8 @@
       <c r="C2" s="2">
         <v>5.5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -1918,12 +1912,8 @@
       <c r="C3" s="1">
         <v>12.5</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
@@ -1935,12 +1925,8 @@
       <c r="C4" s="1">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
@@ -1952,12 +1938,8 @@
       <c r="C5" s="1">
         <v>18.899999999999999</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
@@ -1969,12 +1951,8 @@
       <c r="C6" s="1">
         <v>14.17</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
@@ -2026,12 +2004,8 @@
         <f>(145.17-98.28)/3.92</f>
         <v>11.961734693877547</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -2082,7 +2056,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2115,9 +2089,7 @@
       <c r="C2" s="2">
         <v>16</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -2129,9 +2101,7 @@
       <c r="C3" s="1">
         <v>9</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
@@ -2172,7 +2142,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D3" sqref="D3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2245,9 +2215,7 @@
       <c r="C3" s="1">
         <v>339</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="D3" s="9"/>
       <c r="G3" t="s">
         <v>28</v>
       </c>
@@ -2271,9 +2239,7 @@
       <c r="C4" s="1">
         <v>760</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="D4" s="9"/>
       <c r="G4" t="s">
         <v>28</v>
       </c>
@@ -2297,9 +2263,7 @@
       <c r="C5" s="1">
         <v>770</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="D5" s="9"/>
       <c r="G5" t="s">
         <v>28</v>
       </c>
@@ -2443,8 +2407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2476,9 +2440,7 @@
       <c r="C2" s="2">
         <v>2.09</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -2490,9 +2452,7 @@
       <c r="C3" s="1">
         <v>0.2</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
@@ -2504,9 +2464,7 @@
       <c r="C4" s="1">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
@@ -2518,9 +2476,7 @@
       <c r="C5" s="1">
         <v>0.32</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">

</xml_diff>

<commit_message>
delete "FraselleJacobs1987"'s value from CBM thickness
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A99B3A8-86B0-544D-A779-9EFF33D362F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8A501D-3A98-104A-A616-F89639892FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22920" activeTab="4" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22920" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{64BEA8E4-9BD4-734F-93FA-A8843F7785E6}">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{5B8BC328-C175-1645-944D-85396FC5B1C5}">
       <text>
         <r>
           <rPr>
@@ -417,11 +417,41 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>I caluclated using upper and lower limit.</t>
+          <t xml:space="preserve">SE
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">n = 4
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>=&gt; SD = SE*sqrt(4)</t>
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{5B8BC328-C175-1645-944D-85396FC5B1C5}">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
       <text>
         <r>
           <rPr>
@@ -450,7 +480,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">SE
+          <t xml:space="preserve">We need to check for accuracy
 </t>
         </r>
         <r>
@@ -470,21 +500,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>=&gt; SD = SE*sqrt(4)</t>
+          <t>SD = SE * sqrt(n)</t>
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{182B70E3-48A9-A749-92A6-5153F0941F12}">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{869334AA-FFFD-AE45-94B9-ED3218882153}">
       <text>
         <r>
           <rPr>
@@ -513,104 +533,51 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">We need to check for accuracy
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">n = 4
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>SD = SE * sqrt(n)</t>
+          <t xml:space="preserve">Calculated SE using
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">95% percentile: 194.26
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">5% percentile: 67.23
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Accuracy of calculation is unknown</t>
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{869334AA-FFFD-AE45-94B9-ED3218882153}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yunjeong Lee:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Calculated SE using
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">95% percentile: 194.26
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">5% percentile: 67.23
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Accuracy of calculation is unknown</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{64054238-CC51-B445-B187-AE09C29B0B3E}">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{64054238-CC51-B445-B187-AE09C29B0B3E}">
       <text>
         <r>
           <rPr>
@@ -830,7 +797,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="39">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -872,9 +839,6 @@
   </si>
   <si>
     <t>Lash1989</t>
-  </si>
-  <si>
-    <t>Jacobs1987</t>
   </si>
   <si>
     <t>Belligoli2019</t>
@@ -1580,7 +1544,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1824,7 +1788,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1859,10 +1823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:E9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1880,18 +1844,18 @@
         <v>5</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2">
         <v>69</v>
@@ -1904,7 +1868,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
         <v>56.78</v>
@@ -1917,7 +1881,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <v>73</v>
@@ -1930,7 +1894,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1">
         <v>92.87</v>
@@ -1943,7 +1907,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1">
         <v>76.75</v>
@@ -1994,53 +1958,38 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>89</v>
+      </c>
+      <c r="C9" s="1">
+        <f>B9*2.2/100*2</f>
+        <v>3.9160000000000004</v>
+      </c>
+      <c r="D9" s="1">
+        <v>113.4</v>
+      </c>
+      <c r="E9" s="9">
+        <f>B9*2/100*2</f>
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1">
-        <f>(98.28+145.17)/2</f>
-        <v>121.72499999999999</v>
-      </c>
-      <c r="C9" s="1">
-        <f>(145.17-98.28)/3.92</f>
-        <v>11.961734693877547</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1">
-        <v>89</v>
-      </c>
-      <c r="C10" s="1">
-        <f>B10*2.2/100*2</f>
-        <v>3.9160000000000004</v>
-      </c>
-      <c r="D10" s="1">
-        <v>113.4</v>
-      </c>
-      <c r="E10" s="9">
-        <f>B10*2/100*2</f>
-        <v>3.56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="11">
+      <c r="B10" s="11">
         <v>103.38</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C10" s="11">
         <f>(194.26-67.23)/3.29</f>
         <v>38.610942249240118</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D10" s="11">
         <v>139.87</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E10" s="12">
         <f>(314.612-95.553)/3.29</f>
         <v>66.58328267477205</v>
       </c>
@@ -2070,21 +2019,21 @@
         <v>12</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2">
         <v>16</v>
@@ -2093,10 +2042,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1">
         <v>9</v>
@@ -2105,10 +2054,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -2119,10 +2068,10 @@
     </row>
     <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="11">
         <v>7.5</v>
@@ -2156,33 +2105,33 @@
         <v>12</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>27</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2">
         <f>AVERAGE(I2:I5)</f>
@@ -2193,96 +2142,96 @@
         <v>60.964470527239605</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2">
         <v>340</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1">
         <v>339</v>
       </c>
       <c r="D3" s="9"/>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3">
         <v>110</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1">
         <v>760</v>
       </c>
       <c r="D4" s="9"/>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4">
         <v>330</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1">
         <v>770</v>
       </c>
       <c r="D5" s="9"/>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5">
         <v>140</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1">
         <v>37.1</v>
@@ -2291,24 +2240,24 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I6">
         <v>339</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1">
         <v>51.7</v>
@@ -2317,24 +2266,24 @@
         <v>5.8</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7">
         <v>760</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="11">
         <v>9.8000000000000007</v>
@@ -2343,24 +2292,24 @@
         <v>0.4</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8">
         <v>770</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9">
         <v>37.1</v>
@@ -2371,10 +2320,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10">
         <v>51.7</v>
@@ -2385,10 +2334,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11">
         <v>9.8000000000000007</v>
@@ -2407,7 +2356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3AE235-A997-9D41-BA0F-FEA0B65FE7F6}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
@@ -2421,21 +2370,21 @@
         <v>12</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2">
         <v>2.09</v>
@@ -2444,10 +2393,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1">
         <v>0.2</v>
@@ -2456,10 +2405,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1">
         <v>0.28000000000000003</v>
@@ -2468,10 +2417,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1">
         <v>0.32</v>
@@ -2480,10 +2429,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1">
         <v>113</v>
@@ -2495,10 +2444,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1">
         <v>25</v>
@@ -2509,10 +2458,10 @@
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="11">
         <v>25</v>

</xml_diff>

<commit_message>
delete [Belligoli, 2019]'s data from CBM thickness
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8A501D-3A98-104A-A616-F89639892FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F06E8FA3-F35E-FB47-ABD1-12504C87B383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22400" yWindow="500" windowWidth="22400" windowHeight="22920" activeTab="1" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -504,132 +504,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{869334AA-FFFD-AE45-94B9-ED3218882153}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yunjeong Lee:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Calculated SE using
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">95% percentile: 194.26
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">5% percentile: 67.23
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Accuracy of calculation is unknown</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{64054238-CC51-B445-B187-AE09C29B0B3E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yunjeong Lee:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Calculated SE using
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">95% percentile: 314.612
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>5% percentile: 95.553</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -797,7 +671,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="38">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -839,9 +713,6 @@
   </si>
   <si>
     <t>Lash1989</t>
-  </si>
-  <si>
-    <t>Belligoli2019</t>
   </si>
   <si>
     <t>Danis1993</t>
@@ -1544,7 +1415,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1788,7 +1659,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1823,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE76C8D-43AE-4D4B-BC49-57024CA5FDC4}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:E9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1844,18 +1715,18 @@
         <v>5</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2">
         <v>69</v>
@@ -1868,7 +1739,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>56.78</v>
@@ -1881,7 +1752,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>73</v>
@@ -1894,7 +1765,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>92.87</v>
@@ -1907,7 +1778,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>76.75</v>
@@ -1956,42 +1827,23 @@
         <v>7.4953911286600103</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1">
+    <row r="9" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="11">
         <v>89</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="11">
         <f>B9*2.2/100*2</f>
         <v>3.9160000000000004</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="11">
         <v>113.4</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="12">
         <f>B9*2/100*2</f>
         <v>3.56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="11">
-        <v>103.38</v>
-      </c>
-      <c r="C10" s="11">
-        <f>(194.26-67.23)/3.29</f>
-        <v>38.610942249240118</v>
-      </c>
-      <c r="D10" s="11">
-        <v>139.87</v>
-      </c>
-      <c r="E10" s="12">
-        <f>(314.612-95.553)/3.29</f>
-        <v>66.58328267477205</v>
       </c>
     </row>
   </sheetData>
@@ -2019,21 +1871,21 @@
         <v>12</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2">
         <v>16</v>
@@ -2042,10 +1894,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1">
         <v>9</v>
@@ -2054,10 +1906,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -2068,10 +1920,10 @@
     </row>
     <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="11">
         <v>7.5</v>
@@ -2105,33 +1957,33 @@
         <v>12</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>26</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
         <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2">
         <f>AVERAGE(I2:I5)</f>
@@ -2142,96 +1994,96 @@
         <v>60.964470527239605</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I2">
         <v>340</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1">
         <v>339</v>
       </c>
       <c r="D3" s="9"/>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3">
         <v>110</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1">
         <v>760</v>
       </c>
       <c r="D4" s="9"/>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4">
         <v>330</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1">
         <v>770</v>
       </c>
       <c r="D5" s="9"/>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I5">
         <v>140</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1">
         <v>37.1</v>
@@ -2240,24 +2092,24 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6">
         <v>339</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1">
         <v>51.7</v>
@@ -2266,24 +2118,24 @@
         <v>5.8</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7">
         <v>760</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="11">
         <v>9.8000000000000007</v>
@@ -2292,24 +2144,24 @@
         <v>0.4</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8">
         <v>770</v>
       </c>
       <c r="J8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9">
         <v>37.1</v>
@@ -2320,10 +2172,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10">
         <v>51.7</v>
@@ -2334,10 +2186,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11">
         <v>9.8000000000000007</v>
@@ -2370,21 +2222,21 @@
         <v>12</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2">
         <v>2.09</v>
@@ -2393,10 +2245,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1">
         <v>0.2</v>
@@ -2405,10 +2257,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1">
         <v>0.28000000000000003</v>
@@ -2417,10 +2269,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1">
         <v>0.32</v>
@@ -2429,10 +2281,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1">
         <v>113</v>
@@ -2444,10 +2296,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1">
         <v>25</v>
@@ -2458,10 +2310,10 @@
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="11">
         <v>25</v>

</xml_diff>

<commit_message>
use values using 5 nM recombinant VEGF in (Huang, 1998)
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FA0309-447D-0641-8D02-4CF485F5DA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9210092D-77B7-9E42-A79A-67CF0FC04707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="2340" windowWidth="22400" windowHeight="22920" activeTab="3" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
+    <workbookView xWindow="1120" yWindow="740" windowWidth="22400" windowHeight="16700" activeTab="3" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Adipocyte diameter" sheetId="1" r:id="rId1"/>
@@ -1060,7 +1060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1101,7 +1101,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1947,7 +1946,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1990,12 +1989,12 @@
         <v>29</v>
       </c>
       <c r="C2" s="2">
-        <f>AVERAGE(I2:I5)</f>
-        <v>230</v>
+        <f>AVERAGE(I3,I5)</f>
+        <v>125</v>
       </c>
       <c r="D2" s="7">
-        <f>STDEVA(I2:I5)/SQRT(4)</f>
-        <v>60.964470527239605</v>
+        <f>STDEVA(I3,I5)/SQRT(4)</f>
+        <v>10.606601717798213</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>
@@ -2161,10 +2160,10 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="11">

</xml_diff>

<commit_message>
edit calculation of standard error of (Huang, 1998)
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9210092D-77B7-9E42-A79A-67CF0FC04707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41428CCE-A558-CE4E-98FF-F323F78FF5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="740" windowWidth="22400" windowHeight="16700" activeTab="3" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -1946,7 +1946,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1993,8 +1993,8 @@
         <v>125</v>
       </c>
       <c r="D2" s="7">
-        <f>STDEVA(I3,I5)/SQRT(4)</f>
-        <v>10.606601717798213</v>
+        <f>STDEVA(I3,I5)/SQRT(2)</f>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
use (Huang, 1998) data (VEGF-A165 and VEGF-A164)
</commit_message>
<xml_diff>
--- a/data/parameters.xlsx
+++ b/data/parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeonglee/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/meta-analysis-for-VEGF-signaling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41428CCE-A558-CE4E-98FF-F323F78FF5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4190084A-E821-F240-ACFE-9F9C6E13A482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="740" windowWidth="22400" windowHeight="16700" activeTab="3" xr2:uid="{A8742877-6D88-CF4E-82A9-6C281EC17BAE}"/>
   </bookViews>
@@ -557,7 +557,7 @@
     <author>Yunjeong Lee</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{A124DBD5-EB01-BE49-9F02-CF0382B8ADE1}">
       <text>
         <r>
           <rPr>
@@ -590,7 +590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{104F6701-04B9-E649-AC30-2F7E66E4AB3A}">
       <text>
         <r>
           <rPr>
@@ -671,7 +671,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="50">
   <si>
     <t>Lijnen2006</t>
   </si>
@@ -739,12 +739,6 @@
     <t>Mamer2020</t>
   </si>
   <si>
-    <t>Teran2019</t>
-  </si>
-  <si>
-    <t>Tiedemann2002</t>
-  </si>
-  <si>
     <t>Kd average</t>
   </si>
   <si>
@@ -769,15 +763,6 @@
     <t>Cunningham1999</t>
   </si>
   <si>
-    <t>Soker1996</t>
-  </si>
-  <si>
-    <t>Soker1998</t>
-  </si>
-  <si>
-    <t>Fuh2000</t>
-  </si>
-  <si>
     <t>dr = r/(2A)*dA</t>
   </si>
   <si>
@@ -788,6 +773,54 @@
   </si>
   <si>
     <t>Shobhan2023</t>
+  </si>
+  <si>
+    <t>Whitaker et al., 2001</t>
+  </si>
+  <si>
+    <t>Mamer et al., 2020</t>
+  </si>
+  <si>
+    <t>Shobhan et al., 2023</t>
+  </si>
+  <si>
+    <t>Huang et al., 1998 (VEGF-A165)</t>
+  </si>
+  <si>
+    <t>Huang et al., 1998 (VEGF-A164)</t>
+  </si>
+  <si>
+    <t>Waltenberger et al., 1994 (PAE cell)</t>
+  </si>
+  <si>
+    <t>Waltenberger et al., 1994 (HUVEC)</t>
+  </si>
+  <si>
+    <t>Cunningham et al., 1999 (pre-dimerized)</t>
+  </si>
+  <si>
+    <t>Cunningham et al., 1999 (monomer)</t>
+  </si>
+  <si>
+    <t>Soker et al., 1996 (HUVEC)</t>
+  </si>
+  <si>
+    <t>Soker et al., 1996 (breast cancer cell)</t>
+  </si>
+  <si>
+    <t>Soker et al., 1998</t>
+  </si>
+  <si>
+    <t>Fuh et al., 2000</t>
+  </si>
+  <si>
+    <t>Teran et al., 2019 (chimera)</t>
+  </si>
+  <si>
+    <t>Teran et al., 2019 (monomer)</t>
+  </si>
+  <si>
+    <t>Tiedemann et al., 2002</t>
   </si>
 </sst>
 </file>
@@ -1662,7 +1695,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1718,13 +1751,13 @@
         <v>5</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -1860,7 +1893,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1874,21 +1907,21 @@
         <v>12</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2">
         <v>16</v>
@@ -1897,10 +1930,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1">
         <v>9</v>
@@ -1909,10 +1942,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1923,10 +1956,10 @@
     </row>
     <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="11">
         <v>7.5</v>
@@ -1946,12 +1979,12 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1960,47 +1993,47 @@
         <v>12</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2">
-        <f>AVERAGE(I3,I5)</f>
-        <v>125</v>
+        <f>AVERAGE(I2:I3)</f>
+        <v>225</v>
       </c>
       <c r="D2" s="7">
-        <f>STDEVA(I3,I5)/SQRT(2)</f>
-        <v>15</v>
+        <f>STDEVA(I2:I3)/SQRT(2)</f>
+        <v>115</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I2">
         <v>340</v>
@@ -2010,21 +2043,25 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="1">
-        <v>339</v>
-      </c>
-      <c r="D3" s="9"/>
+      <c r="A3" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2">
+        <f>AVERAGE(I4:I5)</f>
+        <v>235</v>
+      </c>
+      <c r="D3" s="7">
+        <f>STDEVA(I4:I5)/SQRT(2)</f>
+        <v>95</v>
+      </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I3">
         <v>110</v>
@@ -2035,20 +2072,20 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1">
-        <v>760</v>
+        <v>339</v>
       </c>
       <c r="D4" s="9"/>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I4">
         <v>330</v>
@@ -2059,20 +2096,20 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="D5" s="9"/>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I5">
         <v>140</v>
@@ -2083,22 +2120,20 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1">
-        <v>37.1</v>
-      </c>
-      <c r="D6" s="9">
-        <v>4.9000000000000004</v>
-      </c>
+        <v>770</v>
+      </c>
+      <c r="D6" s="9"/>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6">
         <v>339</v>
@@ -2109,22 +2144,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1">
-        <v>51.7</v>
+        <v>37.1</v>
       </c>
       <c r="D7" s="9">
-        <v>5.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G7" t="s">
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I7">
         <v>760</v>
@@ -2135,22 +2170,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
-        <v>9.8000000000000007</v>
+        <v>51.7</v>
       </c>
       <c r="D8" s="9">
-        <v>0.4</v>
+        <v>5.8</v>
       </c>
       <c r="G8" t="s">
         <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I8">
         <v>770</v>
@@ -2159,40 +2194,52 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="G9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="11">
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9">
+        <v>37.1</v>
+      </c>
+      <c r="J9">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="11">
         <f>AVERAGE(I12:I14)</f>
         <v>580</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D10" s="12">
         <f>STDEVA(I12:I14)/SQRT(3)</f>
         <v>156.31165450257808</v>
       </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="G10" t="s">
         <v>29</v>
       </c>
-      <c r="I9">
-        <v>37.1</v>
-      </c>
-      <c r="J9">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G10" t="s">
-        <v>31</v>
-      </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I10">
         <v>51.7</v>
@@ -2206,7 +2253,7 @@
         <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I11">
         <v>9.8000000000000007</v>
@@ -2217,10 +2264,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I12">
         <v>700</v>
@@ -2228,10 +2275,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I13">
         <v>770</v>
@@ -2239,10 +2286,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I14">
         <v>270</v>
@@ -2259,12 +2306,12 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2272,21 +2319,21 @@
         <v>12</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2">
         <v>2.09</v>
@@ -2295,10 +2342,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1">
         <v>0.2</v>
@@ -2307,10 +2354,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1">
         <v>0.28000000000000003</v>
@@ -2319,10 +2366,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1">
         <v>0.32</v>
@@ -2331,10 +2378,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1">
         <v>113</v>
@@ -2346,10 +2393,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1">
         <v>25</v>
@@ -2360,10 +2407,10 @@
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="11">
         <v>25</v>

</xml_diff>